<commit_message>
change product_details table columns type
</commit_message>
<xml_diff>
--- a/public/sample-format/roaming-operator-excel.xlsx
+++ b/public/sample-format/roaming-operator-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp2\htdocs\bl_cms\public\sample-format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23673842-B2E4-482D-8183-D842F2F03B5B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE45F25E-13FF-4BA5-BA24-28AF6891A65A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8B35BE1C-AA5A-4CD2-933C-CCC4D98FA47E}"/>
   </bookViews>
@@ -1694,7 +1694,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{878BF039-E789-487E-BAA7-427DB46C30B7}">
   <dimension ref="A1:E3005"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>